<commit_message>
datos de importacion 2
</commit_message>
<xml_diff>
--- a/Datos de Importacion.xlsx
+++ b/Datos de Importacion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="16368" windowHeight="5352"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="16368" windowHeight="5352"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>Compaña</t>
   </si>
   <si>
-    <t>JORDI</t>
-  </si>
-  <si>
     <t>IDENTIFICACION</t>
   </si>
   <si>
@@ -47,15 +44,9 @@
     <t>Telefno</t>
   </si>
   <si>
-    <t>2494-0687</t>
-  </si>
-  <si>
     <t>Direcicon</t>
   </si>
   <si>
-    <t>Diagonal a Perimercados Grecia centro</t>
-  </si>
-  <si>
     <t>Period o</t>
   </si>
   <si>
@@ -68,15 +59,9 @@
     <t>email</t>
   </si>
   <si>
-    <t>joyeriajordi.g@gmail.com</t>
-  </si>
-  <si>
     <t>pas</t>
   </si>
   <si>
-    <t>Gjoyeriajordi1</t>
-  </si>
-  <si>
     <t>smto</t>
   </si>
   <si>
@@ -87,6 +72,21 @@
   </si>
   <si>
     <t>tls</t>
+  </si>
+  <si>
+    <t>D' SANTI</t>
+  </si>
+  <si>
+    <t>2445-8293</t>
+  </si>
+  <si>
+    <t>200m Sur Urgencias Hospital San Ramon</t>
+  </si>
+  <si>
+    <t>dsanti.srm@gmail.com</t>
+  </si>
+  <si>
+    <t>Srmdsanti2</t>
   </si>
 </sst>
 </file>
@@ -428,44 +428,44 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -473,39 +473,39 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>587</v>
@@ -513,12 +513,13 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>